<commit_message>
Prod testing errors fixed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_OnboardingRegistration_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A540F10E-E313-443F-8D8C-3252B5A68534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C776C7F9-31D7-4E39-BFC9-BA29E0258ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="14745" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="1440" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,96 @@
   </si>
   <si>
     <t>Shared</t>
+  </si>
+  <si>
+    <t>12_ArriveNowCredentials</t>
+  </si>
+  <si>
+    <t>ArriveNowCredentials</t>
+  </si>
+  <si>
+    <t>12_ArriveNowURL</t>
+  </si>
+  <si>
+    <t>12_ArrivePortalURL</t>
+  </si>
+  <si>
+    <t>12_ArriveTruckEntryURL</t>
+  </si>
+  <si>
+    <t>12_EmailAddress</t>
+  </si>
+  <si>
+    <t>12_GDriveReportFolder</t>
+  </si>
+  <si>
+    <t>12_ToEmail</t>
+  </si>
+  <si>
+    <t>12_CCEmail</t>
+  </si>
+  <si>
+    <t>ArriveNowURL</t>
+  </si>
+  <si>
+    <t>ArrivePortalURL</t>
+  </si>
+  <si>
+    <t>ArriveTruckEntryURL</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>GDriveReportFolder</t>
+  </si>
+  <si>
+    <t>ToEmail</t>
+  </si>
+  <si>
+    <t>CCEmail</t>
+  </si>
+  <si>
+    <t>12_ArriveCarrierSearchURL</t>
+  </si>
+  <si>
+    <t>ArriveCarrierSearchURL</t>
+  </si>
+  <si>
+    <t>Credentials to login into ArriveNow Portal</t>
+  </si>
+  <si>
+    <t>URL for ArriveNow Portal</t>
+  </si>
+  <si>
+    <t>URL for Arrive Portal</t>
+  </si>
+  <si>
+    <t>URL for ArriveNow Truck Entry Portal</t>
+  </si>
+  <si>
+    <t>URL for ArriveNow Carrier Search Portal</t>
+  </si>
+  <si>
+    <t>Email account used to send and create report files</t>
+  </si>
+  <si>
+    <t>ID for G Drive folder where reports are stored</t>
+  </si>
+  <si>
+    <t>Email addresses where the emails are going to be sent to</t>
+  </si>
+  <si>
+    <t>Email addresses copied to the emails that are going to be sent</t>
+  </si>
+  <si>
+    <t>12_ReportFileID</t>
+  </si>
+  <si>
+    <t>ReportFileID</t>
+  </si>
+  <si>
+    <t>ID for G Sheet used to report execution outputs</t>
   </si>
 </sst>
 </file>
@@ -2784,7 +2874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2830,16 +2922,146 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Version ready for testing. Scenario 1 tested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_OnboardingRegistration_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C776C7F9-31D7-4E39-BFC9-BA29E0258ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8708D5C-DB23-4FBD-B068-0798327C711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1440" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="1605" windowWidth="21600" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -162,94 +162,148 @@
     <t>Shared</t>
   </si>
   <si>
+    <t>12_ArriveNowURL</t>
+  </si>
+  <si>
+    <t>12_ArrivePortalURL</t>
+  </si>
+  <si>
+    <t>12_ArriveTruckEntryURL</t>
+  </si>
+  <si>
+    <t>12_GDriveReportFolder</t>
+  </si>
+  <si>
+    <t>12_ToEmail</t>
+  </si>
+  <si>
+    <t>12_CCEmail</t>
+  </si>
+  <si>
+    <t>ArriveNowURL</t>
+  </si>
+  <si>
+    <t>ArrivePortalURL</t>
+  </si>
+  <si>
+    <t>ArriveTruckEntryURL</t>
+  </si>
+  <si>
+    <t>GDriveReportFolder</t>
+  </si>
+  <si>
+    <t>ToEmail</t>
+  </si>
+  <si>
+    <t>CCEmail</t>
+  </si>
+  <si>
+    <t>12_ArriveCarrierSearchURL</t>
+  </si>
+  <si>
+    <t>ArriveCarrierSearchURL</t>
+  </si>
+  <si>
+    <t>URL for ArriveNow Portal</t>
+  </si>
+  <si>
+    <t>URL for Arrive Portal</t>
+  </si>
+  <si>
+    <t>URL for ArriveNow Truck Entry Portal</t>
+  </si>
+  <si>
+    <t>URL for ArriveNow Carrier Search Portal</t>
+  </si>
+  <si>
+    <t>ID for G Drive folder where reports are stored</t>
+  </si>
+  <si>
+    <t>Email addresses where the emails are going to be sent to</t>
+  </si>
+  <si>
+    <t>Email addresses copied to the emails that are going to be sent</t>
+  </si>
+  <si>
+    <t>12_ReportFileID</t>
+  </si>
+  <si>
+    <t>ReportFileID</t>
+  </si>
+  <si>
+    <t>ID for G Sheet used to report execution outputs</t>
+  </si>
+  <si>
+    <t>ReportCreationDate</t>
+  </si>
+  <si>
+    <t>12_ReportCreationDate</t>
+  </si>
+  <si>
+    <t>Date used to check when the last report was created</t>
+  </si>
+  <si>
+    <t>12_ReportFileURL</t>
+  </si>
+  <si>
+    <t>ReportFileURL</t>
+  </si>
+  <si>
+    <t>URL for G Sheet used to report execution outputs</t>
+  </si>
+  <si>
+    <t>CompletedCasesCount</t>
+  </si>
+  <si>
+    <t>ExceptionCasesCount</t>
+  </si>
+  <si>
+    <t>12_CompletedCasesCount</t>
+  </si>
+  <si>
+    <t>12_ExceptionCasesCount</t>
+  </si>
+  <si>
+    <t>This asset holds the number of completed cases for the day</t>
+  </si>
+  <si>
+    <t>This asset holds the number of exception cases for the day</t>
+  </si>
+  <si>
+    <t>MasterReportID</t>
+  </si>
+  <si>
+    <t>12_MasterReportID</t>
+  </si>
+  <si>
+    <t>MasterReportURL</t>
+  </si>
+  <si>
+    <t>12_MasterReportURL</t>
+  </si>
+  <si>
+    <t>ID for G Sheet for the Master execution report</t>
+  </si>
+  <si>
+    <t>URL for G Sheet for the Master execution report</t>
+  </si>
+  <si>
+    <t>TotalCasesCount</t>
+  </si>
+  <si>
+    <t>12_TotalCasesCount</t>
+  </si>
+  <si>
+    <t>This asset holds the number of cases processed for the day</t>
+  </si>
+  <si>
+    <t>ArriveNow_CredentialName</t>
+  </si>
+  <si>
+    <t>The name of the orchestrator asset where the ArriveNow credentials are stored</t>
+  </si>
+  <si>
     <t>12_ArriveNowCredentials</t>
-  </si>
-  <si>
-    <t>ArriveNowCredentials</t>
-  </si>
-  <si>
-    <t>12_ArriveNowURL</t>
-  </si>
-  <si>
-    <t>12_ArrivePortalURL</t>
-  </si>
-  <si>
-    <t>12_ArriveTruckEntryURL</t>
-  </si>
-  <si>
-    <t>12_EmailAddress</t>
-  </si>
-  <si>
-    <t>12_GDriveReportFolder</t>
-  </si>
-  <si>
-    <t>12_ToEmail</t>
-  </si>
-  <si>
-    <t>12_CCEmail</t>
-  </si>
-  <si>
-    <t>ArriveNowURL</t>
-  </si>
-  <si>
-    <t>ArrivePortalURL</t>
-  </si>
-  <si>
-    <t>ArriveTruckEntryURL</t>
-  </si>
-  <si>
-    <t>EmailAddress</t>
-  </si>
-  <si>
-    <t>GDriveReportFolder</t>
-  </si>
-  <si>
-    <t>ToEmail</t>
-  </si>
-  <si>
-    <t>CCEmail</t>
-  </si>
-  <si>
-    <t>12_ArriveCarrierSearchURL</t>
-  </si>
-  <si>
-    <t>ArriveCarrierSearchURL</t>
-  </si>
-  <si>
-    <t>Credentials to login into ArriveNow Portal</t>
-  </si>
-  <si>
-    <t>URL for ArriveNow Portal</t>
-  </si>
-  <si>
-    <t>URL for Arrive Portal</t>
-  </si>
-  <si>
-    <t>URL for ArriveNow Truck Entry Portal</t>
-  </si>
-  <si>
-    <t>URL for ArriveNow Carrier Search Portal</t>
-  </si>
-  <si>
-    <t>Email account used to send and create report files</t>
-  </si>
-  <si>
-    <t>ID for G Drive folder where reports are stored</t>
-  </si>
-  <si>
-    <t>Email addresses where the emails are going to be sent to</t>
-  </si>
-  <si>
-    <t>Email addresses copied to the emails that are going to be sent</t>
-  </si>
-  <si>
-    <t>12_ReportFileID</t>
-  </si>
-  <si>
-    <t>ReportFileID</t>
-  </si>
-  <si>
-    <t>ID for G Sheet used to report execution outputs</t>
   </si>
 </sst>
 </file>
@@ -329,9 +383,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -369,7 +423,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -475,7 +529,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -617,7 +671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -707,7 +761,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2872,10 +2936,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2924,7 +2988,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
@@ -2933,119 +2997,119 @@
         <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -3062,11 +3126,76 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4049,8 +4178,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated logic to enter the scheduled lanes on the new MOB section in ANow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_OnboardingRegistration_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1C13B3-9ABC-43E7-B61F-04BDCB7D6824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB77580-C5AC-4B82-BA72-F93497F91601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -313,6 +313,15 @@
   </si>
   <si>
     <t>This asset holds the amount of runtime of the RPA</t>
+  </si>
+  <si>
+    <t>ArriveMOBURL</t>
+  </si>
+  <si>
+    <t>12_ArriveMOBURL</t>
+  </si>
+  <si>
+    <t>URL for Arrive Match Offer Book</t>
   </si>
 </sst>
 </file>
@@ -2948,7 +2957,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3219,7 +3228,20 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+    </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>